<commit_message>
Double checked analyses. Added a supplement file with taxonomic informaiton.
</commit_message>
<xml_diff>
--- a/Taxonomy information/Invertebrate_taxonomy_corrected.xlsx
+++ b/Taxonomy information/Invertebrate_taxonomy_corrected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gamtostyrimai-my.sharepoint.com/personal/nathan_baker_gamtc_lt/Documents/Breitenbach/Breitenbach_2.0_revised/Taxonomy information/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gamtostyrimai-my.sharepoint.com/personal/nathan_baker_gamtc_lt/Documents/Breitenbach/Breitenbach_2.0/Taxonomy information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1882" documentId="11_52B98414FCFA48855B20FB2F63CC0B385FEB635F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B080126-1E00-4AAD-9D48-B95D94507DFC}"/>
+  <xr:revisionPtr revIDLastSave="1884" documentId="11_52B98414FCFA48855B20FB2F63CC0B385FEB635F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD3DED23-9E0E-42F3-A253-A3E68D33622C}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Corrected taxonomy" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Corrected taxonomy'!$A$1:$Y$1004</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Diptera_taxonomy_cleaned!$A$1:$H$518</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Other_taxonomy_cleaned!$A$1:$H$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Other_taxonomy_cleaned!$A$1:$H$133</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Taxonomy_cleaned!$A$1:$H$650</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -70041,9 +70041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224FF961-7CEE-4F24-8D40-8C809427B162}">
   <dimension ref="A1:H518"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A320" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G518"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -83539,9 +83539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31401F2-12D8-4392-BB0E-5CA67242C5B9}">
   <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -87014,7 +87014,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H127" xr:uid="{D31401F2-12D8-4392-BB0E-5CA67242C5B9}"/>
+  <autoFilter ref="A1:H133" xr:uid="{D31401F2-12D8-4392-BB0E-5CA67242C5B9}"/>
   <conditionalFormatting sqref="H1:H127 D1:D127 D134:D1048576 H134:H1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>

</xml_diff>